<commit_message>
added no repeating courses. I think I have other courses loaded
</commit_message>
<xml_diff>
--- a/csp_course_rotations.xlsx
+++ b/csp_course_rotations.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/szczurpi/Google Drive/LewisU/Data Science/Course Schedules/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christian\Desktop\Master\School\2020\Fall\CPSC57100\Week_6\Mp3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24E755D8-7F3D-3045-9E2C-20E9D608B6BC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A3BA6B9-55A9-487A-83EC-CE546ADDB2AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="2060" windowWidth="27640" windowHeight="16940" xr2:uid="{CD2308FA-6A06-1D48-B40D-6494088EB855}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{CD2308FA-6A06-1D48-B40D-6494088EB855}"/>
   </bookViews>
   <sheets>
     <sheet name="course_rotations" sheetId="1" r:id="rId1"/>
     <sheet name="prereqs" sheetId="2" r:id="rId2"/>
+    <sheet name="course_rotations_4_years" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="36">
   <si>
     <t>CPSC-50100</t>
   </si>
@@ -104,13 +105,43 @@
   </si>
   <si>
     <t>capstone</t>
+  </si>
+  <si>
+    <t>Fall 1</t>
+  </si>
+  <si>
+    <t>Fall 2</t>
+  </si>
+  <si>
+    <t>Spring 1</t>
+  </si>
+  <si>
+    <t>Spring 2</t>
+  </si>
+  <si>
+    <t>Summer 1</t>
+  </si>
+  <si>
+    <t>Summer 2</t>
+  </si>
+  <si>
+    <t>Year 1</t>
+  </si>
+  <si>
+    <t>Year 2</t>
+  </si>
+  <si>
+    <t>Year 3</t>
+  </si>
+  <si>
+    <t>Year 4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -132,16 +163,46 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -164,16 +225,108 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -490,16 +643,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E50D480-F901-B547-8C6B-03EE5B95BB51}">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H19" sqref="A1:H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="13.83203125" customWidth="1"/>
+    <col min="1" max="2" width="13.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -525,7 +678,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -551,7 +704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -577,7 +730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -603,7 +756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -629,7 +782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -655,7 +808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -681,7 +834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -707,7 +860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -733,7 +886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -759,7 +912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -785,7 +938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -811,7 +964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -837,7 +990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -863,7 +1016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -889,7 +1042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -915,7 +1068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -941,7 +1094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -967,7 +1120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1006,13 +1159,13 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.1640625" customWidth="1"/>
-    <col min="2" max="2" width="16.83203125" customWidth="1"/>
+    <col min="1" max="1" width="16.125" customWidth="1"/>
+    <col min="2" max="2" width="16.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -1020,7 +1173,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1028,7 +1181,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1036,7 +1189,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -1044,7 +1197,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -1052,7 +1205,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -1060,7 +1213,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -1068,7 +1221,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -1076,7 +1229,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -1084,7 +1237,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -1092,7 +1245,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -1100,7 +1253,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -1108,7 +1261,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -1116,7 +1269,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -1124,7 +1277,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>1</v>
       </c>
@@ -1132,7 +1285,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -1140,7 +1293,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -1148,7 +1301,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>0</v>
       </c>
@@ -1156,7 +1309,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -1164,7 +1317,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>5</v>
       </c>
@@ -1172,7 +1325,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>6</v>
       </c>
@@ -1180,7 +1333,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -1188,7 +1341,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>8</v>
       </c>
@@ -1199,4 +1352,1763 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20A2A377-EE1B-484C-A30E-8B48AC4C11ED}">
+  <dimension ref="A1:AA21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.125" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="7" max="7" width="8.875" customWidth="1"/>
+    <col min="8" max="8" width="11.125" customWidth="1"/>
+    <col min="9" max="9" width="12.5" customWidth="1"/>
+    <col min="14" max="14" width="11.125" customWidth="1"/>
+    <col min="15" max="15" width="11.75" customWidth="1"/>
+    <col min="20" max="20" width="12.5" customWidth="1"/>
+    <col min="21" max="21" width="11.875" customWidth="1"/>
+    <col min="26" max="26" width="11.125" customWidth="1"/>
+    <col min="27" max="27" width="10.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="M1" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="N1" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="O1" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="P1" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q1" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="R1" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="S1" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="T1" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="U1" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="V1" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="W1" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="X1" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y1" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z1" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA1" s="33" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="L2" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="M2" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="N2" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="O2" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="P2" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q2" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="R2" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="S2" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="T2" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="U2" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="V2" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="W2" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="X2" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y2" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z2" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA2" s="33" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8"/>
+      <c r="B3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="39">
+        <v>1</v>
+      </c>
+      <c r="E3" s="20">
+        <v>2</v>
+      </c>
+      <c r="F3" s="20">
+        <v>3</v>
+      </c>
+      <c r="G3" s="20">
+        <v>4</v>
+      </c>
+      <c r="H3" s="20">
+        <v>5</v>
+      </c>
+      <c r="I3" s="25">
+        <v>6</v>
+      </c>
+      <c r="J3" s="21">
+        <v>7</v>
+      </c>
+      <c r="K3" s="21">
+        <v>8</v>
+      </c>
+      <c r="L3" s="21">
+        <v>9</v>
+      </c>
+      <c r="M3" s="21">
+        <v>10</v>
+      </c>
+      <c r="N3" s="21">
+        <v>11</v>
+      </c>
+      <c r="O3" s="28">
+        <v>12</v>
+      </c>
+      <c r="P3" s="22">
+        <v>13</v>
+      </c>
+      <c r="Q3" s="22">
+        <v>14</v>
+      </c>
+      <c r="R3" s="22">
+        <v>15</v>
+      </c>
+      <c r="S3" s="22">
+        <v>16</v>
+      </c>
+      <c r="T3" s="22">
+        <v>17</v>
+      </c>
+      <c r="U3" s="31">
+        <v>18</v>
+      </c>
+      <c r="V3" s="23">
+        <v>19</v>
+      </c>
+      <c r="W3" s="23">
+        <v>20</v>
+      </c>
+      <c r="X3" s="23">
+        <v>21</v>
+      </c>
+      <c r="Y3" s="23">
+        <v>22</v>
+      </c>
+      <c r="Z3" s="23">
+        <v>23</v>
+      </c>
+      <c r="AA3" s="34">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
+        <v>1</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="5">
+        <v>1</v>
+      </c>
+      <c r="E4" s="5">
+        <v>1</v>
+      </c>
+      <c r="F4" s="5">
+        <v>1</v>
+      </c>
+      <c r="G4" s="5">
+        <v>0</v>
+      </c>
+      <c r="H4" s="5">
+        <v>1</v>
+      </c>
+      <c r="I4" s="26">
+        <v>0</v>
+      </c>
+      <c r="J4" s="6">
+        <v>1</v>
+      </c>
+      <c r="K4" s="6">
+        <v>1</v>
+      </c>
+      <c r="L4" s="6">
+        <v>1</v>
+      </c>
+      <c r="M4" s="6">
+        <v>0</v>
+      </c>
+      <c r="N4" s="6">
+        <v>1</v>
+      </c>
+      <c r="O4" s="29">
+        <v>0</v>
+      </c>
+      <c r="P4" s="18">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="18">
+        <v>1</v>
+      </c>
+      <c r="R4" s="18">
+        <v>1</v>
+      </c>
+      <c r="S4" s="18">
+        <v>0</v>
+      </c>
+      <c r="T4" s="18">
+        <v>1</v>
+      </c>
+      <c r="U4" s="32">
+        <v>0</v>
+      </c>
+      <c r="V4" s="19">
+        <v>1</v>
+      </c>
+      <c r="W4" s="19">
+        <v>1</v>
+      </c>
+      <c r="X4" s="19">
+        <v>1</v>
+      </c>
+      <c r="Y4" s="19">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="19">
+        <v>1</v>
+      </c>
+      <c r="AA4" s="35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="9">
+        <v>2</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="10">
+        <v>1</v>
+      </c>
+      <c r="E5" s="10">
+        <v>0</v>
+      </c>
+      <c r="F5" s="10">
+        <v>1</v>
+      </c>
+      <c r="G5" s="10">
+        <v>0</v>
+      </c>
+      <c r="H5" s="10">
+        <v>1</v>
+      </c>
+      <c r="I5" s="24">
+        <v>0</v>
+      </c>
+      <c r="J5" s="11">
+        <v>1</v>
+      </c>
+      <c r="K5" s="11">
+        <v>0</v>
+      </c>
+      <c r="L5" s="11">
+        <v>1</v>
+      </c>
+      <c r="M5" s="11">
+        <v>0</v>
+      </c>
+      <c r="N5" s="11">
+        <v>1</v>
+      </c>
+      <c r="O5" s="27">
+        <v>0</v>
+      </c>
+      <c r="P5" s="12">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="12">
+        <v>0</v>
+      </c>
+      <c r="R5" s="12">
+        <v>1</v>
+      </c>
+      <c r="S5" s="12">
+        <v>0</v>
+      </c>
+      <c r="T5" s="12">
+        <v>1</v>
+      </c>
+      <c r="U5" s="30">
+        <v>0</v>
+      </c>
+      <c r="V5" s="13">
+        <v>1</v>
+      </c>
+      <c r="W5" s="13">
+        <v>0</v>
+      </c>
+      <c r="X5" s="13">
+        <v>1</v>
+      </c>
+      <c r="Y5" s="13">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="13">
+        <v>1</v>
+      </c>
+      <c r="AA5" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="9">
+        <v>3</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="10">
+        <v>0</v>
+      </c>
+      <c r="E6" s="10">
+        <v>1</v>
+      </c>
+      <c r="F6" s="10">
+        <v>0</v>
+      </c>
+      <c r="G6" s="10">
+        <v>1</v>
+      </c>
+      <c r="H6" s="10">
+        <v>0</v>
+      </c>
+      <c r="I6" s="24">
+        <v>0</v>
+      </c>
+      <c r="J6" s="11">
+        <v>0</v>
+      </c>
+      <c r="K6" s="11">
+        <v>1</v>
+      </c>
+      <c r="L6" s="11">
+        <v>0</v>
+      </c>
+      <c r="M6" s="11">
+        <v>1</v>
+      </c>
+      <c r="N6" s="11">
+        <v>0</v>
+      </c>
+      <c r="O6" s="27">
+        <v>0</v>
+      </c>
+      <c r="P6" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="12">
+        <v>1</v>
+      </c>
+      <c r="R6" s="12">
+        <v>0</v>
+      </c>
+      <c r="S6" s="12">
+        <v>1</v>
+      </c>
+      <c r="T6" s="12">
+        <v>0</v>
+      </c>
+      <c r="U6" s="30">
+        <v>0</v>
+      </c>
+      <c r="V6" s="13">
+        <v>0</v>
+      </c>
+      <c r="W6" s="13">
+        <v>1</v>
+      </c>
+      <c r="X6" s="13">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="13">
+        <v>1</v>
+      </c>
+      <c r="Z6" s="13">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="9">
+        <v>4</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="10">
+        <v>0</v>
+      </c>
+      <c r="E7" s="10">
+        <v>0</v>
+      </c>
+      <c r="F7" s="10">
+        <v>0</v>
+      </c>
+      <c r="G7" s="10">
+        <v>1</v>
+      </c>
+      <c r="H7" s="10">
+        <v>0</v>
+      </c>
+      <c r="I7" s="24">
+        <v>0</v>
+      </c>
+      <c r="J7" s="11">
+        <v>0</v>
+      </c>
+      <c r="K7" s="11">
+        <v>0</v>
+      </c>
+      <c r="L7" s="11">
+        <v>0</v>
+      </c>
+      <c r="M7" s="11">
+        <v>1</v>
+      </c>
+      <c r="N7" s="11">
+        <v>0</v>
+      </c>
+      <c r="O7" s="27">
+        <v>0</v>
+      </c>
+      <c r="P7" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="12">
+        <v>0</v>
+      </c>
+      <c r="R7" s="12">
+        <v>0</v>
+      </c>
+      <c r="S7" s="12">
+        <v>1</v>
+      </c>
+      <c r="T7" s="12">
+        <v>0</v>
+      </c>
+      <c r="U7" s="30">
+        <v>0</v>
+      </c>
+      <c r="V7" s="13">
+        <v>0</v>
+      </c>
+      <c r="W7" s="13">
+        <v>0</v>
+      </c>
+      <c r="X7" s="13">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="13">
+        <v>1</v>
+      </c>
+      <c r="Z7" s="13">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="9">
+        <v>5</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="10">
+        <v>1</v>
+      </c>
+      <c r="E8" s="10">
+        <v>0</v>
+      </c>
+      <c r="F8" s="10">
+        <v>0</v>
+      </c>
+      <c r="G8" s="10">
+        <v>0</v>
+      </c>
+      <c r="H8" s="10">
+        <v>1</v>
+      </c>
+      <c r="I8" s="24">
+        <v>0</v>
+      </c>
+      <c r="J8" s="11">
+        <v>1</v>
+      </c>
+      <c r="K8" s="11">
+        <v>0</v>
+      </c>
+      <c r="L8" s="11">
+        <v>0</v>
+      </c>
+      <c r="M8" s="11">
+        <v>0</v>
+      </c>
+      <c r="N8" s="11">
+        <v>1</v>
+      </c>
+      <c r="O8" s="27">
+        <v>0</v>
+      </c>
+      <c r="P8" s="12">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="12">
+        <v>0</v>
+      </c>
+      <c r="R8" s="12">
+        <v>0</v>
+      </c>
+      <c r="S8" s="12">
+        <v>0</v>
+      </c>
+      <c r="T8" s="12">
+        <v>1</v>
+      </c>
+      <c r="U8" s="30">
+        <v>0</v>
+      </c>
+      <c r="V8" s="13">
+        <v>1</v>
+      </c>
+      <c r="W8" s="13">
+        <v>0</v>
+      </c>
+      <c r="X8" s="13">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="13">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="13">
+        <v>1</v>
+      </c>
+      <c r="AA8" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="9">
+        <v>6</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="10">
+        <v>1</v>
+      </c>
+      <c r="E9" s="10">
+        <v>0</v>
+      </c>
+      <c r="F9" s="10">
+        <v>1</v>
+      </c>
+      <c r="G9" s="10">
+        <v>0</v>
+      </c>
+      <c r="H9" s="10">
+        <v>1</v>
+      </c>
+      <c r="I9" s="24">
+        <v>0</v>
+      </c>
+      <c r="J9" s="11">
+        <v>1</v>
+      </c>
+      <c r="K9" s="11">
+        <v>0</v>
+      </c>
+      <c r="L9" s="11">
+        <v>1</v>
+      </c>
+      <c r="M9" s="11">
+        <v>0</v>
+      </c>
+      <c r="N9" s="11">
+        <v>1</v>
+      </c>
+      <c r="O9" s="27">
+        <v>0</v>
+      </c>
+      <c r="P9" s="12">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="12">
+        <v>0</v>
+      </c>
+      <c r="R9" s="12">
+        <v>1</v>
+      </c>
+      <c r="S9" s="12">
+        <v>0</v>
+      </c>
+      <c r="T9" s="12">
+        <v>1</v>
+      </c>
+      <c r="U9" s="30">
+        <v>0</v>
+      </c>
+      <c r="V9" s="13">
+        <v>1</v>
+      </c>
+      <c r="W9" s="13">
+        <v>0</v>
+      </c>
+      <c r="X9" s="13">
+        <v>1</v>
+      </c>
+      <c r="Y9" s="13">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="13">
+        <v>1</v>
+      </c>
+      <c r="AA9" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="9">
+        <v>7</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="10">
+        <v>0</v>
+      </c>
+      <c r="E10" s="10">
+        <v>1</v>
+      </c>
+      <c r="F10" s="10">
+        <v>0</v>
+      </c>
+      <c r="G10" s="10">
+        <v>0</v>
+      </c>
+      <c r="H10" s="10">
+        <v>1</v>
+      </c>
+      <c r="I10" s="24">
+        <v>0</v>
+      </c>
+      <c r="J10" s="11">
+        <v>0</v>
+      </c>
+      <c r="K10" s="11">
+        <v>1</v>
+      </c>
+      <c r="L10" s="11">
+        <v>0</v>
+      </c>
+      <c r="M10" s="11">
+        <v>0</v>
+      </c>
+      <c r="N10" s="11">
+        <v>1</v>
+      </c>
+      <c r="O10" s="27">
+        <v>0</v>
+      </c>
+      <c r="P10" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="12">
+        <v>1</v>
+      </c>
+      <c r="R10" s="12">
+        <v>0</v>
+      </c>
+      <c r="S10" s="12">
+        <v>0</v>
+      </c>
+      <c r="T10" s="12">
+        <v>1</v>
+      </c>
+      <c r="U10" s="30">
+        <v>0</v>
+      </c>
+      <c r="V10" s="13">
+        <v>0</v>
+      </c>
+      <c r="W10" s="13">
+        <v>1</v>
+      </c>
+      <c r="X10" s="13">
+        <v>0</v>
+      </c>
+      <c r="Y10" s="13">
+        <v>0</v>
+      </c>
+      <c r="Z10" s="13">
+        <v>1</v>
+      </c>
+      <c r="AA10" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="8">
+        <v>8</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="5">
+        <v>0</v>
+      </c>
+      <c r="E11" s="5">
+        <v>1</v>
+      </c>
+      <c r="F11" s="5">
+        <v>1</v>
+      </c>
+      <c r="G11" s="5">
+        <v>0</v>
+      </c>
+      <c r="H11" s="5">
+        <v>0</v>
+      </c>
+      <c r="I11" s="26">
+        <v>0</v>
+      </c>
+      <c r="J11" s="6">
+        <v>0</v>
+      </c>
+      <c r="K11" s="6">
+        <v>1</v>
+      </c>
+      <c r="L11" s="6">
+        <v>1</v>
+      </c>
+      <c r="M11" s="6">
+        <v>0</v>
+      </c>
+      <c r="N11" s="6">
+        <v>0</v>
+      </c>
+      <c r="O11" s="29">
+        <v>0</v>
+      </c>
+      <c r="P11" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="18">
+        <v>1</v>
+      </c>
+      <c r="R11" s="18">
+        <v>1</v>
+      </c>
+      <c r="S11" s="18">
+        <v>0</v>
+      </c>
+      <c r="T11" s="18">
+        <v>0</v>
+      </c>
+      <c r="U11" s="32">
+        <v>0</v>
+      </c>
+      <c r="V11" s="19">
+        <v>0</v>
+      </c>
+      <c r="W11" s="19">
+        <v>1</v>
+      </c>
+      <c r="X11" s="19">
+        <v>1</v>
+      </c>
+      <c r="Y11" s="19">
+        <v>0</v>
+      </c>
+      <c r="Z11" s="19">
+        <v>0</v>
+      </c>
+      <c r="AA11" s="35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="9">
+        <v>9</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="10">
+        <v>1</v>
+      </c>
+      <c r="E12" s="10">
+        <v>0</v>
+      </c>
+      <c r="F12" s="10">
+        <v>0</v>
+      </c>
+      <c r="G12" s="10">
+        <v>0</v>
+      </c>
+      <c r="H12" s="10">
+        <v>1</v>
+      </c>
+      <c r="I12" s="24">
+        <v>0</v>
+      </c>
+      <c r="J12" s="11">
+        <v>1</v>
+      </c>
+      <c r="K12" s="11">
+        <v>0</v>
+      </c>
+      <c r="L12" s="11">
+        <v>0</v>
+      </c>
+      <c r="M12" s="11">
+        <v>0</v>
+      </c>
+      <c r="N12" s="11">
+        <v>1</v>
+      </c>
+      <c r="O12" s="27">
+        <v>0</v>
+      </c>
+      <c r="P12" s="12">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="12">
+        <v>0</v>
+      </c>
+      <c r="R12" s="12">
+        <v>0</v>
+      </c>
+      <c r="S12" s="12">
+        <v>0</v>
+      </c>
+      <c r="T12" s="12">
+        <v>1</v>
+      </c>
+      <c r="U12" s="30">
+        <v>0</v>
+      </c>
+      <c r="V12" s="13">
+        <v>1</v>
+      </c>
+      <c r="W12" s="13">
+        <v>0</v>
+      </c>
+      <c r="X12" s="13">
+        <v>0</v>
+      </c>
+      <c r="Y12" s="13">
+        <v>0</v>
+      </c>
+      <c r="Z12" s="13">
+        <v>1</v>
+      </c>
+      <c r="AA12" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="9">
+        <v>10</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="10">
+        <v>1</v>
+      </c>
+      <c r="E13" s="10">
+        <v>0</v>
+      </c>
+      <c r="F13" s="10">
+        <v>1</v>
+      </c>
+      <c r="G13" s="10">
+        <v>0</v>
+      </c>
+      <c r="H13" s="10">
+        <v>1</v>
+      </c>
+      <c r="I13" s="24">
+        <v>0</v>
+      </c>
+      <c r="J13" s="11">
+        <v>1</v>
+      </c>
+      <c r="K13" s="11">
+        <v>0</v>
+      </c>
+      <c r="L13" s="11">
+        <v>1</v>
+      </c>
+      <c r="M13" s="11">
+        <v>0</v>
+      </c>
+      <c r="N13" s="11">
+        <v>1</v>
+      </c>
+      <c r="O13" s="27">
+        <v>0</v>
+      </c>
+      <c r="P13" s="12">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="12">
+        <v>0</v>
+      </c>
+      <c r="R13" s="12">
+        <v>1</v>
+      </c>
+      <c r="S13" s="12">
+        <v>0</v>
+      </c>
+      <c r="T13" s="12">
+        <v>1</v>
+      </c>
+      <c r="U13" s="30">
+        <v>0</v>
+      </c>
+      <c r="V13" s="13">
+        <v>1</v>
+      </c>
+      <c r="W13" s="13">
+        <v>0</v>
+      </c>
+      <c r="X13" s="13">
+        <v>1</v>
+      </c>
+      <c r="Y13" s="13">
+        <v>0</v>
+      </c>
+      <c r="Z13" s="13">
+        <v>1</v>
+      </c>
+      <c r="AA13" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="9">
+        <v>11</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="10">
+        <v>0</v>
+      </c>
+      <c r="E14" s="10">
+        <v>1</v>
+      </c>
+      <c r="F14" s="10">
+        <v>0</v>
+      </c>
+      <c r="G14" s="10">
+        <v>0</v>
+      </c>
+      <c r="H14" s="10">
+        <v>0</v>
+      </c>
+      <c r="I14" s="24">
+        <v>0</v>
+      </c>
+      <c r="J14" s="11">
+        <v>0</v>
+      </c>
+      <c r="K14" s="11">
+        <v>1</v>
+      </c>
+      <c r="L14" s="11">
+        <v>0</v>
+      </c>
+      <c r="M14" s="11">
+        <v>0</v>
+      </c>
+      <c r="N14" s="11">
+        <v>0</v>
+      </c>
+      <c r="O14" s="27">
+        <v>0</v>
+      </c>
+      <c r="P14" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="12">
+        <v>1</v>
+      </c>
+      <c r="R14" s="12">
+        <v>0</v>
+      </c>
+      <c r="S14" s="12">
+        <v>0</v>
+      </c>
+      <c r="T14" s="12">
+        <v>0</v>
+      </c>
+      <c r="U14" s="30">
+        <v>0</v>
+      </c>
+      <c r="V14" s="13">
+        <v>0</v>
+      </c>
+      <c r="W14" s="13">
+        <v>1</v>
+      </c>
+      <c r="X14" s="13">
+        <v>0</v>
+      </c>
+      <c r="Y14" s="13">
+        <v>0</v>
+      </c>
+      <c r="Z14" s="13">
+        <v>0</v>
+      </c>
+      <c r="AA14" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="9">
+        <v>12</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="10">
+        <v>0</v>
+      </c>
+      <c r="E15" s="10">
+        <v>1</v>
+      </c>
+      <c r="F15" s="10">
+        <v>0</v>
+      </c>
+      <c r="G15" s="10">
+        <v>1</v>
+      </c>
+      <c r="H15" s="10">
+        <v>0</v>
+      </c>
+      <c r="I15" s="24">
+        <v>1</v>
+      </c>
+      <c r="J15" s="11">
+        <v>0</v>
+      </c>
+      <c r="K15" s="11">
+        <v>1</v>
+      </c>
+      <c r="L15" s="11">
+        <v>0</v>
+      </c>
+      <c r="M15" s="11">
+        <v>1</v>
+      </c>
+      <c r="N15" s="11">
+        <v>0</v>
+      </c>
+      <c r="O15" s="27">
+        <v>1</v>
+      </c>
+      <c r="P15" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="12">
+        <v>1</v>
+      </c>
+      <c r="R15" s="12">
+        <v>0</v>
+      </c>
+      <c r="S15" s="12">
+        <v>1</v>
+      </c>
+      <c r="T15" s="12">
+        <v>0</v>
+      </c>
+      <c r="U15" s="30">
+        <v>1</v>
+      </c>
+      <c r="V15" s="13">
+        <v>0</v>
+      </c>
+      <c r="W15" s="13">
+        <v>1</v>
+      </c>
+      <c r="X15" s="13">
+        <v>0</v>
+      </c>
+      <c r="Y15" s="13">
+        <v>1</v>
+      </c>
+      <c r="Z15" s="13">
+        <v>0</v>
+      </c>
+      <c r="AA15" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="9">
+        <v>13</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="10">
+        <v>0</v>
+      </c>
+      <c r="E16" s="10">
+        <v>1</v>
+      </c>
+      <c r="F16" s="10">
+        <v>0</v>
+      </c>
+      <c r="G16" s="10">
+        <v>0</v>
+      </c>
+      <c r="H16" s="10">
+        <v>0</v>
+      </c>
+      <c r="I16" s="24">
+        <v>0</v>
+      </c>
+      <c r="J16" s="11">
+        <v>0</v>
+      </c>
+      <c r="K16" s="11">
+        <v>1</v>
+      </c>
+      <c r="L16" s="11">
+        <v>0</v>
+      </c>
+      <c r="M16" s="11">
+        <v>0</v>
+      </c>
+      <c r="N16" s="11">
+        <v>0</v>
+      </c>
+      <c r="O16" s="27">
+        <v>0</v>
+      </c>
+      <c r="P16" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="12">
+        <v>1</v>
+      </c>
+      <c r="R16" s="12">
+        <v>0</v>
+      </c>
+      <c r="S16" s="12">
+        <v>0</v>
+      </c>
+      <c r="T16" s="12">
+        <v>0</v>
+      </c>
+      <c r="U16" s="30">
+        <v>0</v>
+      </c>
+      <c r="V16" s="13">
+        <v>0</v>
+      </c>
+      <c r="W16" s="13">
+        <v>1</v>
+      </c>
+      <c r="X16" s="13">
+        <v>0</v>
+      </c>
+      <c r="Y16" s="13">
+        <v>0</v>
+      </c>
+      <c r="Z16" s="13">
+        <v>0</v>
+      </c>
+      <c r="AA16" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="9">
+        <v>14</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="10">
+        <v>1</v>
+      </c>
+      <c r="E17" s="10">
+        <v>0</v>
+      </c>
+      <c r="F17" s="10">
+        <v>0</v>
+      </c>
+      <c r="G17" s="10">
+        <v>1</v>
+      </c>
+      <c r="H17" s="10">
+        <v>0</v>
+      </c>
+      <c r="I17" s="24">
+        <v>0</v>
+      </c>
+      <c r="J17" s="11">
+        <v>1</v>
+      </c>
+      <c r="K17" s="11">
+        <v>0</v>
+      </c>
+      <c r="L17" s="11">
+        <v>0</v>
+      </c>
+      <c r="M17" s="11">
+        <v>1</v>
+      </c>
+      <c r="N17" s="11">
+        <v>0</v>
+      </c>
+      <c r="O17" s="27">
+        <v>0</v>
+      </c>
+      <c r="P17" s="12">
+        <v>1</v>
+      </c>
+      <c r="Q17" s="12">
+        <v>0</v>
+      </c>
+      <c r="R17" s="12">
+        <v>0</v>
+      </c>
+      <c r="S17" s="12">
+        <v>1</v>
+      </c>
+      <c r="T17" s="12">
+        <v>0</v>
+      </c>
+      <c r="U17" s="30">
+        <v>0</v>
+      </c>
+      <c r="V17" s="13">
+        <v>1</v>
+      </c>
+      <c r="W17" s="13">
+        <v>0</v>
+      </c>
+      <c r="X17" s="13">
+        <v>0</v>
+      </c>
+      <c r="Y17" s="13">
+        <v>1</v>
+      </c>
+      <c r="Z17" s="13">
+        <v>0</v>
+      </c>
+      <c r="AA17" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="9">
+        <v>15</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="10">
+        <v>0</v>
+      </c>
+      <c r="E18" s="10">
+        <v>0</v>
+      </c>
+      <c r="F18" s="10">
+        <v>1</v>
+      </c>
+      <c r="G18" s="10">
+        <v>0</v>
+      </c>
+      <c r="H18" s="10">
+        <v>0</v>
+      </c>
+      <c r="I18" s="24">
+        <v>0</v>
+      </c>
+      <c r="J18" s="11">
+        <v>0</v>
+      </c>
+      <c r="K18" s="11">
+        <v>0</v>
+      </c>
+      <c r="L18" s="11">
+        <v>1</v>
+      </c>
+      <c r="M18" s="11">
+        <v>0</v>
+      </c>
+      <c r="N18" s="11">
+        <v>0</v>
+      </c>
+      <c r="O18" s="27">
+        <v>0</v>
+      </c>
+      <c r="P18" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="12">
+        <v>0</v>
+      </c>
+      <c r="R18" s="12">
+        <v>1</v>
+      </c>
+      <c r="S18" s="12">
+        <v>0</v>
+      </c>
+      <c r="T18" s="12">
+        <v>0</v>
+      </c>
+      <c r="U18" s="30">
+        <v>0</v>
+      </c>
+      <c r="V18" s="13">
+        <v>0</v>
+      </c>
+      <c r="W18" s="13">
+        <v>0</v>
+      </c>
+      <c r="X18" s="13">
+        <v>1</v>
+      </c>
+      <c r="Y18" s="13">
+        <v>0</v>
+      </c>
+      <c r="Z18" s="13">
+        <v>0</v>
+      </c>
+      <c r="AA18" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="9">
+        <v>16</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="10">
+        <v>0</v>
+      </c>
+      <c r="E19" s="10">
+        <v>0</v>
+      </c>
+      <c r="F19" s="10">
+        <v>0</v>
+      </c>
+      <c r="G19" s="10">
+        <v>0</v>
+      </c>
+      <c r="H19" s="10">
+        <v>1</v>
+      </c>
+      <c r="I19" s="24">
+        <v>0</v>
+      </c>
+      <c r="J19" s="11">
+        <v>0</v>
+      </c>
+      <c r="K19" s="11">
+        <v>0</v>
+      </c>
+      <c r="L19" s="11">
+        <v>0</v>
+      </c>
+      <c r="M19" s="11">
+        <v>0</v>
+      </c>
+      <c r="N19" s="11">
+        <v>1</v>
+      </c>
+      <c r="O19" s="27">
+        <v>0</v>
+      </c>
+      <c r="P19" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="12">
+        <v>0</v>
+      </c>
+      <c r="R19" s="12">
+        <v>0</v>
+      </c>
+      <c r="S19" s="12">
+        <v>0</v>
+      </c>
+      <c r="T19" s="12">
+        <v>1</v>
+      </c>
+      <c r="U19" s="30">
+        <v>0</v>
+      </c>
+      <c r="V19" s="13">
+        <v>0</v>
+      </c>
+      <c r="W19" s="13">
+        <v>0</v>
+      </c>
+      <c r="X19" s="13">
+        <v>0</v>
+      </c>
+      <c r="Y19" s="13">
+        <v>0</v>
+      </c>
+      <c r="Z19" s="13">
+        <v>1</v>
+      </c>
+      <c r="AA19" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="9">
+        <v>17</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" s="10">
+        <v>0</v>
+      </c>
+      <c r="E20" s="10">
+        <v>0</v>
+      </c>
+      <c r="F20" s="10">
+        <v>0</v>
+      </c>
+      <c r="G20" s="14">
+        <v>1</v>
+      </c>
+      <c r="H20" s="10">
+        <v>0</v>
+      </c>
+      <c r="I20" s="24">
+        <v>0</v>
+      </c>
+      <c r="J20" s="11">
+        <v>0</v>
+      </c>
+      <c r="K20" s="11">
+        <v>0</v>
+      </c>
+      <c r="L20" s="11">
+        <v>0</v>
+      </c>
+      <c r="M20" s="15">
+        <v>1</v>
+      </c>
+      <c r="N20" s="11">
+        <v>0</v>
+      </c>
+      <c r="O20" s="27">
+        <v>0</v>
+      </c>
+      <c r="P20" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="12">
+        <v>0</v>
+      </c>
+      <c r="R20" s="12">
+        <v>0</v>
+      </c>
+      <c r="S20" s="16">
+        <v>1</v>
+      </c>
+      <c r="T20" s="12">
+        <v>0</v>
+      </c>
+      <c r="U20" s="30">
+        <v>0</v>
+      </c>
+      <c r="V20" s="13">
+        <v>0</v>
+      </c>
+      <c r="W20" s="13">
+        <v>0</v>
+      </c>
+      <c r="X20" s="13">
+        <v>0</v>
+      </c>
+      <c r="Y20" s="17">
+        <v>1</v>
+      </c>
+      <c r="Z20" s="13">
+        <v>0</v>
+      </c>
+      <c r="AA20" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="9">
+        <v>18</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" s="10">
+        <v>0</v>
+      </c>
+      <c r="E21" s="10">
+        <v>1</v>
+      </c>
+      <c r="F21" s="10">
+        <v>0</v>
+      </c>
+      <c r="G21" s="10">
+        <v>1</v>
+      </c>
+      <c r="H21" s="10">
+        <v>1</v>
+      </c>
+      <c r="I21" s="24">
+        <v>0</v>
+      </c>
+      <c r="J21" s="11">
+        <v>0</v>
+      </c>
+      <c r="K21" s="11">
+        <v>1</v>
+      </c>
+      <c r="L21" s="11">
+        <v>0</v>
+      </c>
+      <c r="M21" s="11">
+        <v>1</v>
+      </c>
+      <c r="N21" s="11">
+        <v>1</v>
+      </c>
+      <c r="O21" s="27">
+        <v>0</v>
+      </c>
+      <c r="P21" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="12">
+        <v>1</v>
+      </c>
+      <c r="R21" s="12">
+        <v>0</v>
+      </c>
+      <c r="S21" s="12">
+        <v>1</v>
+      </c>
+      <c r="T21" s="12">
+        <v>1</v>
+      </c>
+      <c r="U21" s="30">
+        <v>0</v>
+      </c>
+      <c r="V21" s="13">
+        <v>0</v>
+      </c>
+      <c r="W21" s="13">
+        <v>1</v>
+      </c>
+      <c r="X21" s="13">
+        <v>0</v>
+      </c>
+      <c r="Y21" s="13">
+        <v>1</v>
+      </c>
+      <c r="Z21" s="13">
+        <v>1</v>
+      </c>
+      <c r="AA21" s="33">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added all but electives
</commit_message>
<xml_diff>
--- a/csp_course_rotations.xlsx
+++ b/csp_course_rotations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christian\Desktop\Master\School\2020\Fall\CPSC57100\Week_6\Mp3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75FAB03F-CA65-42C4-AF7C-CEB820A6370B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C80C9290-CEDF-47B6-8603-261409850E26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{CD2308FA-6A06-1D48-B40D-6494088EB855}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="36">
   <si>
     <t>CPSC-50100</t>
   </si>
@@ -645,7 +645,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A2:A3"/>
+      <selection activeCell="A18" sqref="A11:A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1154,10 +1154,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E1636DF-E6CD-4716-A946-E6E54DB58895}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1176,10 +1176,114 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1191,7 +1295,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD43A1E0-A219-3A44-9ECC-205CE11146B0}">
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="A2:B23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>